<commit_message>
Calling it good enough for now
</commit_message>
<xml_diff>
--- a/currStorm.xlsx
+++ b/currStorm.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
   <si>
     <t xml:space="preserve">Main Copies</t>
   </si>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Past in Flames</t>
   </si>
   <si>
-    <t xml:space="preserve">Krosan Grip</t>
+    <t xml:space="preserve">Hurkyl’s Recall</t>
   </si>
   <si>
     <t xml:space="preserve">BUG Midrange</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">Rain of Filth</t>
   </si>
   <si>
-    <t xml:space="preserve">Hurkyl’s Recall</t>
+    <t xml:space="preserve">Massacre</t>
   </si>
   <si>
     <t xml:space="preserve">BUG Combo</t>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">Thoughtseize</t>
   </si>
   <si>
-    <t xml:space="preserve">Massecre</t>
+    <t xml:space="preserve">Echoing Truth</t>
   </si>
   <si>
     <t xml:space="preserve">UR (No Wasteland)</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">Preordain</t>
   </si>
   <si>
-    <t xml:space="preserve">Echoing Truth</t>
+    <t xml:space="preserve">Xantid Swarm</t>
   </si>
   <si>
     <t xml:space="preserve">Grixis Control</t>
@@ -124,16 +124,13 @@
     <t xml:space="preserve">Preordain!</t>
   </si>
   <si>
-    <t xml:space="preserve">Xantid Swarm</t>
+    <t xml:space="preserve">Fatal Push</t>
   </si>
   <si>
     <t xml:space="preserve">Burn</t>
   </si>
   <si>
     <t xml:space="preserve">Lotus Petal!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fatal Push</t>
   </si>
   <si>
     <t xml:space="preserve">UB Reanimator</t>
@@ -308,7 +305,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -326,6 +323,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -449,19 +454,21 @@
   </sheetPr>
   <dimension ref="A1:BP65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7125506072875"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9959514170041"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.99595141700405"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.7125506072875"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,51 +491,51 @@
       <c r="G1" s="0"/>
       <c r="H1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,H3:H37)/SUM($G3:$G37)</f>
-        <v>2.34</v>
+        <v>3.25</v>
       </c>
       <c r="I1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,I3:I37)/SUM($G3:$G37)</f>
-        <v>1.95</v>
+        <v>2.54</v>
       </c>
       <c r="J1" s="0" t="n">
-        <f aca="false">SUMPRODUCT($G3:$G37,J40:J74)/SUM($G3:$G37)</f>
-        <v>2.97</v>
+        <f aca="false">SUMPRODUCT($G3:$G37,J3:J37)/SUM($G3:$G37)</f>
+        <v>4.4</v>
       </c>
       <c r="K1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,K3:K37)/SUM($G3:$G37)</f>
-        <v>2.31</v>
+        <v>3.36</v>
       </c>
       <c r="L1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,L3:L37)/SUM($G3:$G37)</f>
-        <v>2.03</v>
+        <v>2.63</v>
       </c>
       <c r="M1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,M3:M37)/SUM($G3:$G37)</f>
-        <v>2.1</v>
+        <v>2.84</v>
       </c>
       <c r="N1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,N3:N37)/SUM($G3:$G37)</f>
-        <v>1.51</v>
+        <v>1.99</v>
       </c>
       <c r="O1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,O3:O37)/SUM($G3:$G37)</f>
-        <v>1.52</v>
+        <v>1.82</v>
       </c>
       <c r="P1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,P3:P37)/SUM($G3:$G37)</f>
-        <v>1.5</v>
+        <v>2.74</v>
       </c>
       <c r="Q1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,Q3:Q37)/SUM($G3:$G37)</f>
-        <v>2.14</v>
+        <v>2.18</v>
       </c>
       <c r="R1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,R3:R37)/SUM($G3:$G37)</f>
-        <v>1.65</v>
+        <v>1.95</v>
       </c>
       <c r="S1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,S3:S37)/SUM($G3:$G37)</f>
-        <v>1.46</v>
+        <v>0</v>
       </c>
       <c r="T1" s="0" t="n">
         <f aca="false">SUMPRODUCT($G3:$G37,T3:T37)/SUM($G3:$G37)</f>
@@ -588,30 +595,30 @@
       </c>
       <c r="N2" s="1" t="str">
         <f aca="false">D8</f>
-        <v>Krosan Grip</v>
+        <v>Hurkyl’s Recall</v>
       </c>
       <c r="O2" s="1" t="str">
         <f aca="false">$D$9</f>
-        <v>Hurkyl’s Recall</v>
+        <v>Massacre</v>
       </c>
       <c r="P2" s="1" t="str">
         <f aca="false">$D$10</f>
-        <v>Massecre</v>
+        <v>Echoing Truth</v>
       </c>
       <c r="Q2" s="1" t="str">
         <f aca="false">D11</f>
-        <v>Echoing Truth</v>
+        <v>Xantid Swarm</v>
       </c>
       <c r="R2" s="1" t="str">
         <f aca="false">D12</f>
-        <v>Xantid Swarm</v>
-      </c>
-      <c r="S2" s="1" t="str">
+        <v>Fatal Push</v>
+      </c>
+      <c r="S2" s="1" t="n">
         <f aca="false">D13</f>
-        <v>Fatal Push</v>
+        <v>0</v>
       </c>
       <c r="T2" s="1" t="n">
-        <f aca="false">D14</f>
+        <f aca="false">D13</f>
         <v>0</v>
       </c>
       <c r="U2" s="1" t="n">
@@ -646,23 +653,23 @@
         <v>1</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J3" s="0" t="n">
         <f aca="false">J40</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>1</v>
@@ -671,12 +678,9 @@
         <v>1</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="S3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -703,17 +707,17 @@
         <v>1</v>
       </c>
       <c r="I4" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J4" s="0" t="n">
         <f aca="false">J41</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>1</v>
@@ -722,19 +726,16 @@
         <v>1</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="S4" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,17 +758,17 @@
         <v>6</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5" s="0" t="n">
         <f aca="false">J42</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>1</v>
@@ -776,21 +777,18 @@
         <v>1</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q5" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -821,16 +819,16 @@
       </c>
       <c r="J6" s="0" t="n">
         <f aca="false">J43</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M6" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>1</v>
@@ -845,9 +843,6 @@
         <v>1</v>
       </c>
       <c r="R6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -871,14 +866,14 @@
         <v>4</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J7" s="0" t="n">
         <f aca="false">J44</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>1</v>
@@ -890,21 +885,18 @@
         <v>1</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -916,7 +908,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>22</v>
@@ -931,20 +923,20 @@
         <v>1</v>
       </c>
       <c r="I8" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J8" s="0" t="n">
         <f aca="false">J45</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="M8" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>1</v>
@@ -959,9 +951,6 @@
         <v>1</v>
       </c>
       <c r="R8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S8" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -973,9 +962,9 @@
         <v>24</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="0" t="s">
@@ -988,11 +977,11 @@
         <v>1</v>
       </c>
       <c r="I9" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J9" s="0" t="n">
         <f aca="false">J46</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>1</v>
@@ -1016,9 +1005,6 @@
         <v>1</v>
       </c>
       <c r="R9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S9" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1030,9 +1016,9 @@
         <v>27</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>28</v>
       </c>
       <c r="F10" s="0" t="s">
@@ -1045,14 +1031,14 @@
         <v>1</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J10" s="0" t="n">
         <f aca="false">J47</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L10" s="0" t="n">
         <v>2</v>
@@ -1073,9 +1059,6 @@
         <v>1</v>
       </c>
       <c r="R10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S10" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1087,7 +1070,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>31</v>
@@ -1106,16 +1089,16 @@
       </c>
       <c r="J11" s="0" t="n">
         <f aca="false">J48</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M11" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N11" s="0" t="n">
         <v>1</v>
@@ -1127,12 +1110,9 @@
         <v>1</v>
       </c>
       <c r="Q11" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R11" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="S11" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1144,7 +1124,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>34</v>
@@ -1156,7 +1136,7 @@
         <v>3</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>1</v>
@@ -1166,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>1</v>
@@ -1181,16 +1161,13 @@
         <v>1</v>
       </c>
       <c r="P12" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q12" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S12" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1200,14 +1177,8 @@
       <c r="B13" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>1</v>
@@ -1220,16 +1191,16 @@
       </c>
       <c r="J13" s="0" t="n">
         <f aca="false">J50</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N13" s="0" t="n">
         <v>1</v>
@@ -1241,31 +1212,28 @@
         <v>1</v>
       </c>
       <c r="Q13" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="R13" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="S13" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F14" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>3</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>3</v>
       </c>
       <c r="J14" s="0" t="n">
         <f aca="false">J51</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>1</v>
@@ -1274,7 +1242,7 @@
         <v>2</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N14" s="0" t="n">
         <v>1</v>
@@ -1286,24 +1254,21 @@
         <v>1</v>
       </c>
       <c r="Q14" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="R14" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="S14" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="0" t="n">
         <v>8</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>2</v>
@@ -1313,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L15" s="0" t="n">
         <v>1</v>
@@ -1322,97 +1287,91 @@
         <v>1</v>
       </c>
       <c r="N15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O15" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P15" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q15" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S15" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F16" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J16" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H16" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I16" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J16" s="6" t="n">
         <f aca="false">J53</f>
         <v>2</v>
       </c>
-      <c r="K16" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O16" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="R16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S16" s="0" t="n">
+      <c r="K16" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="L16" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="O16" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P16" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q16" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R16" s="6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>5</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J17" s="0" t="n">
         <f aca="false">J54</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M17" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N17" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O17" s="0" t="n">
         <v>1</v>
@@ -1421,31 +1380,28 @@
         <v>1</v>
       </c>
       <c r="Q17" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="R17" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="S17" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J18" s="0" t="n">
         <f aca="false">J55</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K18" s="0" t="n">
         <v>1</v>
@@ -1454,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="M18" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>1</v>
@@ -1469,15 +1425,12 @@
         <v>1</v>
       </c>
       <c r="R18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S18" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F19" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>1</v>
@@ -1490,13 +1443,13 @@
       </c>
       <c r="J19" s="0" t="n">
         <f aca="false">J56</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K19" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M19" s="0" t="n">
         <v>1</v>
@@ -1511,40 +1464,37 @@
         <v>1</v>
       </c>
       <c r="Q19" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R19" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="S19" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="5" t="n">
+      <c r="F20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J20" s="0" t="n">
         <f aca="false">J57</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M20" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N20" s="0" t="n">
         <v>1</v>
@@ -1553,37 +1503,35 @@
         <v>1</v>
       </c>
       <c r="P20" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q20" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="R20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S20" s="5" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="R20" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S20" s="0"/>
     </row>
     <row r="21" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="5" t="n">
+      <c r="F21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="7" t="n">
         <v>8</v>
       </c>
       <c r="H21" s="0" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J21" s="0" t="n">
         <f aca="false">J58</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L21" s="0" t="n">
         <v>2</v>
@@ -1603,29 +1551,27 @@
       <c r="Q21" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="R21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S21" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="5" t="n">
+      <c r="R21" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S21" s="0"/>
+    </row>
+    <row r="22" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="7" t="n">
         <v>1</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I22" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J22" s="0" t="n">
         <f aca="false">J59</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K22" s="0" t="n">
         <v>2</v>
@@ -1640,91 +1586,86 @@
         <v>4</v>
       </c>
       <c r="O22" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P22" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q22" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="R22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S22" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R22" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S22" s="0"/>
+    </row>
+    <row r="23" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H23" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I23" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J23" s="6" t="n">
+        <f aca="false">J60</f>
+        <v>3</v>
+      </c>
+      <c r="K23" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="L23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N23" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="O23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P23" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="R23" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="H23" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <f aca="false">J60</f>
-        <v>2</v>
-      </c>
-      <c r="K23" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="L23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O23" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="P23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="R23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S23" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="5" t="n">
+      <c r="G24" s="7" t="n">
         <v>3</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J24" s="0" t="n">
         <f aca="false">J61</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K24" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L24" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M24" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N24" s="0" t="n">
         <v>1</v>
@@ -1738,22 +1679,20 @@
       <c r="Q24" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="R24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S24" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="5" t="n">
+      <c r="R24" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S24" s="0"/>
+    </row>
+    <row r="25" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="7" t="n">
         <v>4</v>
       </c>
       <c r="H25" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>1</v>
@@ -1769,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="M25" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N25" s="0" t="n">
         <v>1</v>
@@ -1778,37 +1717,35 @@
         <v>1</v>
       </c>
       <c r="P25" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q25" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="R25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="S25" s="5" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="R25" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F26" s="5" t="s">
-        <v>51</v>
+      <c r="F26" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="G26" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>2</v>
       </c>
       <c r="J26" s="0" t="n">
         <f aca="false">J63</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K26" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L26" s="0" t="n">
         <v>1</v>
@@ -1817,40 +1754,37 @@
         <v>1</v>
       </c>
       <c r="N26" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O26" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P26" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q26" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S26" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F27" s="5" t="s">
-        <v>52</v>
+      <c r="F27" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="G27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>2</v>
       </c>
       <c r="J27" s="0" t="n">
         <f aca="false">J64</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K27" s="0" t="n">
         <v>1</v>
@@ -1862,33 +1796,30 @@
         <v>1</v>
       </c>
       <c r="N27" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P27" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q27" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R27" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S27" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F28" s="5" t="s">
-        <v>53</v>
+      <c r="F28" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="G28" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>2</v>
@@ -1898,7 +1829,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L28" s="0" t="n">
         <v>1</v>
@@ -1910,30 +1841,27 @@
         <v>1</v>
       </c>
       <c r="O28" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P28" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Q28" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R28" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S28" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F29" s="5" t="s">
-        <v>54</v>
+      <c r="F29" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>1</v>
@@ -1943,13 +1871,13 @@
         <v>2</v>
       </c>
       <c r="K29" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L29" s="0" t="n">
         <v>1</v>
       </c>
       <c r="M29" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N29" s="0" t="n">
         <v>1</v>
@@ -1958,27 +1886,24 @@
         <v>1</v>
       </c>
       <c r="P29" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q29" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S29" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="5" t="s">
-        <v>55</v>
+      <c r="F30" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>1</v>
@@ -2003,37 +1928,34 @@
         <v>1</v>
       </c>
       <c r="P30" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q30" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R30" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S30" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="5" t="s">
-        <v>56</v>
+      <c r="F31" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="G31" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H31" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I31" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J31" s="0" t="n">
         <f aca="false">J68</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K31" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L31" s="0" t="n">
         <v>1</v>
@@ -2045,24 +1967,21 @@
         <v>4</v>
       </c>
       <c r="O31" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P31" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q31" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R31" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S31" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="5" t="s">
-        <v>57</v>
+      <c r="F32" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>1</v>
@@ -2075,16 +1994,16 @@
       </c>
       <c r="J32" s="0" t="n">
         <f aca="false">J69</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M32" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N32" s="0" t="n">
         <v>1</v>
@@ -2096,18 +2015,15 @@
         <v>1</v>
       </c>
       <c r="Q32" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="R32" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="S32" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F33" s="5" t="s">
-        <v>58</v>
+      <c r="F33" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="G33" s="0" t="n">
         <v>1</v>
@@ -2120,7 +2036,7 @@
       </c>
       <c r="J33" s="0" t="n">
         <f aca="false">J70</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K33" s="0" t="n">
         <v>1</v>
@@ -2129,7 +2045,7 @@
         <v>2</v>
       </c>
       <c r="M33" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N33" s="0" t="n">
         <v>1</v>
@@ -2138,27 +2054,24 @@
         <v>1</v>
       </c>
       <c r="P33" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q33" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R33" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S33" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F34" s="5" t="s">
-        <v>59</v>
+      <c r="F34" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="G34" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H34" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>1</v>
@@ -2180,37 +2093,34 @@
         <v>4</v>
       </c>
       <c r="O34" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P34" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q34" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R34" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S34" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F35" s="5" t="s">
-        <v>60</v>
+      <c r="F35" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="G35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="H35" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J35" s="0" t="n">
         <f aca="false">J72</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K35" s="0" t="n">
         <v>1</v>
@@ -2228,21 +2138,18 @@
         <v>1</v>
       </c>
       <c r="P35" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q35" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R35" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S35" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F36" s="5" t="s">
-        <v>61</v>
+      <c r="F36" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>4</v>
@@ -2251,14 +2158,14 @@
         <v>1</v>
       </c>
       <c r="I36" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J36" s="0" t="n">
         <f aca="false">J73</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K36" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L36" s="0" t="n">
         <v>1</v>
@@ -2270,24 +2177,21 @@
         <v>1</v>
       </c>
       <c r="O36" s="0" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P36" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q36" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R36" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="S36" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F37" s="5" t="s">
-        <v>62</v>
+      <c r="F37" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="G37" s="0" t="n">
         <v>1</v>
@@ -2300,16 +2204,16 @@
       </c>
       <c r="J37" s="0" t="n">
         <f aca="false">J74</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L37" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M37" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N37" s="0" t="n">
         <v>1</v>
@@ -2321,17 +2225,14 @@
         <v>1</v>
       </c>
       <c r="Q37" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R37" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="S37" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F38" s="5"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="0"/>
     </row>
     <row r="39" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2598,37 +2499,37 @@
         <v>8</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K40" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="M40" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N40" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="O40" s="5" t="n">
+        <v>6</v>
+      </c>
+      <c r="O40" s="7" t="n">
         <v>1</v>
       </c>
       <c r="P40" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q40" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R40" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S40" s="0" t="n">
         <v>1</v>
@@ -2644,37 +2545,37 @@
         <v>4</v>
       </c>
       <c r="H41" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K41" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L41" s="0" t="n">
         <v>1</v>
       </c>
       <c r="M41" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N41" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O41" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P41" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q41" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R41" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S41" s="0" t="n">
         <v>3</v>
@@ -2690,19 +2591,19 @@
         <v>6</v>
       </c>
       <c r="H42" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I42" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J42" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K42" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L42" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M42" s="0" t="n">
         <v>1</v>
@@ -2711,19 +2612,19 @@
         <v>1</v>
       </c>
       <c r="O42" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P42" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q42" s="0" t="n">
         <v>1</v>
       </c>
       <c r="R42" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S42" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2736,40 +2637,40 @@
         <v>6</v>
       </c>
       <c r="H43" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I43" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J43" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K43" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L43" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M43" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N43" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O43" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P43" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q43" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R43" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S43" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2782,19 +2683,19 @@
         <v>4</v>
       </c>
       <c r="H44" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I44" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J44" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K44" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L44" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M44" s="0" t="n">
         <v>1</v>
@@ -2803,19 +2704,19 @@
         <v>1</v>
       </c>
       <c r="O44" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P44" s="0" t="n">
         <v>2</v>
       </c>
       <c r="Q44" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R44" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S44" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2828,40 +2729,40 @@
         <v>2</v>
       </c>
       <c r="H45" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J45" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K45" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L45" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M45" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N45" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O45" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P45" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q45" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R45" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S45" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2874,40 +2775,40 @@
         <v>1</v>
       </c>
       <c r="H46" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J46" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K46" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L46" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M46" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N46" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O46" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P46" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q46" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R46" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S46" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2920,40 +2821,40 @@
         <v>1</v>
       </c>
       <c r="H47" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I47" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J47" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K47" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L47" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M47" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N47" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O47" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P47" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q47" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R47" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S47" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2966,40 +2867,40 @@
         <v>7</v>
       </c>
       <c r="H48" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="J48" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K48" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="M48" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N48" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O48" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P48" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q48" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R48" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S48" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3015,7 +2916,7 @@
         <v>1</v>
       </c>
       <c r="I49" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J49" s="0" t="n">
         <v>1</v>
@@ -3024,28 +2925,28 @@
         <v>1</v>
       </c>
       <c r="L49" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M49" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N49" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O49" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P49" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q49" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R49" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S49" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3058,40 +2959,40 @@
         <v>1</v>
       </c>
       <c r="H50" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I50" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J50" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K50" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L50" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M50" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N50" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O50" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P50" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q50" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R50" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S50" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3104,40 +3005,40 @@
         <v>3</v>
       </c>
       <c r="H51" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I51" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J51" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K51" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L51" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M51" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N51" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O51" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P51" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q51" s="0" t="n">
         <v>1</v>
       </c>
       <c r="R51" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S51" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3150,19 +3051,19 @@
         <v>8</v>
       </c>
       <c r="H52" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I52" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J52" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="K52" s="5" t="n">
-        <v>4</v>
+      <c r="K52" s="7" t="n">
+        <v>6</v>
       </c>
       <c r="L52" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M52" s="0" t="n">
         <v>1</v>
@@ -3171,19 +3072,19 @@
         <v>1</v>
       </c>
       <c r="O52" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="P52" s="5" t="n">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="P52" s="7" t="n">
+        <v>6</v>
       </c>
       <c r="Q52" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R52" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S52" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3196,19 +3097,19 @@
         <v>2</v>
       </c>
       <c r="H53" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I53" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J53" s="0" t="n">
         <v>2</v>
       </c>
       <c r="K53" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L53" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M53" s="0" t="n">
         <v>1</v>
@@ -3217,19 +3118,19 @@
         <v>1</v>
       </c>
       <c r="O53" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P53" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q53" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R53" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S53" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3242,40 +3143,40 @@
         <v>5</v>
       </c>
       <c r="H54" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I54" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J54" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K54" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L54" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M54" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N54" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O54" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P54" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q54" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R54" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S54" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3288,19 +3189,19 @@
         <v>2</v>
       </c>
       <c r="H55" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I55" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J55" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K55" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L55" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M55" s="0" t="n">
         <v>2</v>
@@ -3312,16 +3213,16 @@
         <v>1</v>
       </c>
       <c r="P55" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q55" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R55" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S55" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3334,40 +3235,40 @@
         <v>1</v>
       </c>
       <c r="H56" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I56" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J56" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K56" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L56" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M56" s="0" t="n">
         <v>2</v>
       </c>
       <c r="N56" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O56" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P56" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q56" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R56" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S56" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3380,25 +3281,25 @@
         <v>1</v>
       </c>
       <c r="H57" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I57" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J57" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K57" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L57" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M57" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N57" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O57" s="0" t="n">
         <v>4</v>
@@ -3407,13 +3308,13 @@
         <v>2</v>
       </c>
       <c r="Q57" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R57" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S57" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3429,37 +3330,37 @@
         <v>1</v>
       </c>
       <c r="I58" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J58" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K58" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L58" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M58" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N58" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O58" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P58" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q58" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R58" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S58" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3472,19 +3373,19 @@
         <v>1</v>
       </c>
       <c r="H59" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I59" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J59" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K59" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L59" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M59" s="0" t="n">
         <v>1</v>
@@ -3496,7 +3397,7 @@
         <v>1</v>
       </c>
       <c r="P59" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q59" s="0" t="n">
         <v>1</v>
@@ -3505,7 +3406,7 @@
         <v>1</v>
       </c>
       <c r="S59" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3518,19 +3419,19 @@
         <v>3</v>
       </c>
       <c r="H60" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I60" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J60" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K60" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L60" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M60" s="0" t="n">
         <v>1</v>
@@ -3539,50 +3440,50 @@
         <v>1</v>
       </c>
       <c r="O60" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P60" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q60" s="0" t="n">
         <v>1</v>
       </c>
       <c r="R60" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S60" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F61" s="1" t="str">
         <f aca="false">F24</f>
-        <v>BR Reanimator </v>
+        <v>BR Reanimator</v>
       </c>
       <c r="G61" s="1" t="n">
         <f aca="false">G24</f>
         <v>3</v>
       </c>
       <c r="H61" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I61" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J61" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K61" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L61" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M61" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N61" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O61" s="0" t="n">
         <v>1</v>
@@ -3591,13 +3492,13 @@
         <v>2</v>
       </c>
       <c r="Q61" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R61" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S61" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3610,19 +3511,19 @@
         <v>4</v>
       </c>
       <c r="H62" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I62" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J62" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K62" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L62" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M62" s="0" t="n">
         <v>1</v>
@@ -3631,19 +3532,19 @@
         <v>1</v>
       </c>
       <c r="O62" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P62" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q62" s="0" t="n">
         <v>4</v>
       </c>
       <c r="R62" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S62" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3656,19 +3557,19 @@
         <v>1</v>
       </c>
       <c r="H63" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I63" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J63" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K63" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L63" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M63" s="0" t="n">
         <v>1</v>
@@ -3677,19 +3578,19 @@
         <v>1</v>
       </c>
       <c r="O63" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P63" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q63" s="0" t="n">
         <v>1</v>
       </c>
       <c r="R63" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S63" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3702,19 +3603,19 @@
         <v>1</v>
       </c>
       <c r="H64" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I64" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J64" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K64" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L64" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M64" s="0" t="n">
         <v>1</v>
@@ -3723,19 +3624,19 @@
         <v>1</v>
       </c>
       <c r="O64" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P64" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q64" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R64" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S64" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3748,19 +3649,19 @@
         <v>2</v>
       </c>
       <c r="H65" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I65" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J65" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K65" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L65" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M65" s="0" t="n">
         <v>1</v>
@@ -3769,19 +3670,19 @@
         <v>1</v>
       </c>
       <c r="O65" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P65" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q65" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R65" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S65" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3794,40 +3695,40 @@
         <v>1</v>
       </c>
       <c r="H66" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I66" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J66" s="0" t="n">
         <v>2</v>
       </c>
       <c r="K66" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L66" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M66" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N66" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O66" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P66" s="0" t="n">
         <v>1</v>
       </c>
       <c r="Q66" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R66" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S66" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3840,40 +3741,40 @@
         <v>1</v>
       </c>
       <c r="H67" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I67" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J67" s="0" t="n">
         <v>1</v>
       </c>
       <c r="K67" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L67" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M67" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N67" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O67" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P67" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q67" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R67" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S67" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3886,19 +3787,19 @@
         <v>1</v>
       </c>
       <c r="H68" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I68" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J68" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K68" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L68" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M68" s="0" t="n">
         <v>2</v>
@@ -3910,7 +3811,7 @@
         <v>1</v>
       </c>
       <c r="P68" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q68" s="0" t="n">
         <v>1</v>
@@ -3919,7 +3820,7 @@
         <v>1</v>
       </c>
       <c r="S68" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3932,40 +3833,40 @@
         <v>1</v>
       </c>
       <c r="H69" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I69" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J69" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K69" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L69" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M69" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N69" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O69" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P69" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q69" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R69" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S69" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3978,22 +3879,22 @@
         <v>1</v>
       </c>
       <c r="H70" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I70" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J70" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K70" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L70" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M70" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N70" s="0" t="n">
         <v>1</v>
@@ -4002,16 +3903,16 @@
         <v>1</v>
       </c>
       <c r="P70" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q70" s="0" t="n">
         <v>1</v>
       </c>
       <c r="R70" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S70" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4024,19 +3925,19 @@
         <v>1</v>
       </c>
       <c r="H71" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I71" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J71" s="0" t="n">
         <v>2</v>
       </c>
       <c r="K71" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L71" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M71" s="0" t="n">
         <v>1</v>
@@ -4045,19 +3946,19 @@
         <v>1</v>
       </c>
       <c r="O71" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P71" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q71" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R71" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S71" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4070,19 +3971,19 @@
         <v>1</v>
       </c>
       <c r="H72" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I72" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J72" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K72" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L72" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M72" s="0" t="n">
         <v>1</v>
@@ -4091,19 +3992,19 @@
         <v>1</v>
       </c>
       <c r="O72" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P72" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q72" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R72" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S72" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4116,40 +4017,40 @@
         <v>4</v>
       </c>
       <c r="H73" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I73" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J73" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K73" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L73" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M73" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N73" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O73" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P73" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q73" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R73" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S73" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4162,22 +4063,22 @@
         <v>1</v>
       </c>
       <c r="H74" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I74" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J74" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K74" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L74" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M74" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N74" s="0" t="n">
         <v>1</v>
@@ -4186,16 +4087,16 @@
         <v>1</v>
       </c>
       <c r="P74" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q74" s="0" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R74" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S74" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>